<commit_message>
creating case for UC name in different cases
</commit_message>
<xml_diff>
--- a/suppxls/Scen_UCs.xlsx
+++ b/suppxls/Scen_UCs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\DemoS_ADV_Stuttgart061118\suppxls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda\Veda_models\Demo_Adv_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA14BC09-C5DA-4628-AA68-2505383B4254}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C26617-AB1F-4EBC-8E79-7B325C472930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{839C8D2E-9453-4DE3-9534-B724417FAD70}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="12735" xr2:uid="{839C8D2E-9453-4DE3-9534-B724417FAD70}"/>
   </bookViews>
   <sheets>
     <sheet name="DH_Low" sheetId="4" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="58">
   <si>
     <t>UC - Each Region/Interperiod</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>~UC_T: 2010</t>
+  </si>
+  <si>
+    <t>UC_DH_MinPROD</t>
   </si>
 </sst>
 </file>
@@ -882,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB890AEA-F77E-48D6-B975-0A94334584B5}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="N8" sqref="N8:O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,12 +997,6 @@
       <c r="M6" s="26">
         <v>-0.1</v>
       </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>15</v>
-      </c>
       <c r="P6" t="s">
         <v>55</v>
       </c>
@@ -1025,6 +1022,17 @@
       </c>
       <c r="L7" s="26">
         <v>-0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>